<commit_message>
Adding test model for forms example
</commit_message>
<xml_diff>
--- a/src/test/resources/rules-form.xlsx
+++ b/src/test/resources/rules-form.xlsx
@@ -1260,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP992"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T8" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AC5" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1816,7 +1816,7 @@
       <c r="AN9" s="4"/>
       <c r="AO9" s="4"/>
     </row>
-    <row r="10" spans="1:42" ht="144">
+    <row r="10" spans="1:42" ht="129.6">
       <c r="A10" s="4"/>
       <c r="B10" s="52"/>
       <c r="C10" s="53">

</xml_diff>

<commit_message>
Adding mail sending feature
</commit_message>
<xml_diff>
--- a/src/test/resources/rules-form.xlsx
+++ b/src/test/resources/rules-form.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="203">
   <si>
     <t>Locale</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Pregunta 2</t>
   </si>
   <si>
-    <t>getQuestions() $1 null, getQuestions().size() $2 0</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>Extraer todas las preguntas del formulario para inyectarlas en el motor y aplicarles las reglas de manera individual</t>
   </si>
   <si>
-    <t>!=,&gt;</t>
-  </si>
-  <si>
     <t>$form.getQuestions()</t>
   </si>
   <si>
@@ -480,9 +474,6 @@
   </si>
   <si>
     <t>RuleTable for errors in form description</t>
-  </si>
-  <si>
-    <t>getOptions() $1 null, getOptions().size() $2 0</t>
   </si>
   <si>
     <t>for(QuestionOption option : $1) {
@@ -894,6 +885,12 @@
 com.araguacaima.braas.core.RuleMessageSuccess,
 java.util.Set,
 java.util.List</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getOptions().size() &gt; $param</t>
+  </si>
+  <si>
+    <t>getQuestions().size() &gt; $param</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1692,9 +1689,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1849,32 +1843,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1883,7 +1861,26 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1891,9 +1888,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2178,28 +2172,28 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="13.2">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="155" t="s">
+      <c r="C2" s="157" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="19"/>
-      <c r="F2" s="157" t="s">
+      <c r="F2" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="157" t="s">
+      <c r="G2" s="155" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="24"/>
-      <c r="I2" s="157" t="s">
+      <c r="I2" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="157" t="s">
+      <c r="J2" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="26" t="s">
@@ -2248,17 +2242,17 @@
       <c r="C5" s="156"/>
       <c r="D5" s="21"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="157" t="s">
+      <c r="G5" s="155" t="s">
         <v>38</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="157" t="s">
+      <c r="I5" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="157" t="s">
+      <c r="J5" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="26" t="s">
@@ -2324,17 +2318,17 @@
       <c r="C9" s="156"/>
       <c r="D9" s="21"/>
       <c r="E9" s="19"/>
-      <c r="F9" s="157" t="s">
+      <c r="F9" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="157" t="s">
+      <c r="G9" s="155" t="s">
         <v>44</v>
       </c>
       <c r="H9" s="24"/>
-      <c r="I9" s="157" t="s">
+      <c r="I9" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="157" t="s">
+      <c r="J9" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="26" t="s">
@@ -2402,17 +2396,17 @@
       <c r="C13" s="156"/>
       <c r="D13" s="21"/>
       <c r="E13" s="19"/>
-      <c r="F13" s="157" t="s">
+      <c r="F13" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="157" t="s">
+      <c r="G13" s="155" t="s">
         <v>52</v>
       </c>
       <c r="H13" s="24"/>
-      <c r="I13" s="157" t="s">
+      <c r="I13" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="157" t="s">
+      <c r="J13" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K13" s="26" t="s">
@@ -2480,17 +2474,17 @@
       <c r="C17" s="156"/>
       <c r="D17" s="21"/>
       <c r="E17" s="19"/>
-      <c r="F17" s="157" t="s">
+      <c r="F17" s="155" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="157" t="s">
+      <c r="G17" s="155" t="s">
         <v>59</v>
       </c>
       <c r="H17" s="24"/>
-      <c r="I17" s="157" t="s">
+      <c r="I17" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="157" t="s">
+      <c r="J17" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K17" s="26" t="s">
@@ -2522,17 +2516,17 @@
       <c r="C19" s="156"/>
       <c r="D19" s="21"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="157" t="s">
+      <c r="F19" s="155" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="157" t="s">
+      <c r="G19" s="155" t="s">
         <v>62</v>
       </c>
       <c r="H19" s="24"/>
-      <c r="I19" s="157" t="s">
+      <c r="I19" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="157" t="s">
+      <c r="J19" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="26" t="s">
@@ -2564,7 +2558,7 @@
       <c r="C21" s="156"/>
       <c r="D21" s="21"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="155" t="s">
         <v>63</v>
       </c>
       <c r="G21" s="22" t="s">
@@ -2612,17 +2606,17 @@
       <c r="C23" s="156"/>
       <c r="D23" s="21"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="155" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="157" t="s">
+      <c r="G23" s="155" t="s">
         <v>67</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="157" t="s">
+      <c r="I23" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="157" t="s">
+      <c r="J23" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="26" t="s">
@@ -2649,28 +2643,28 @@
       <c r="M24" s="26"/>
     </row>
     <row r="25" spans="1:13" ht="13.2">
-      <c r="A25" s="155" t="s">
+      <c r="A25" s="157" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="155" t="s">
+      <c r="B25" s="157" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="155" t="s">
+      <c r="C25" s="157" t="s">
         <v>70</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="19"/>
-      <c r="F25" s="157" t="s">
+      <c r="F25" s="155" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="157" t="s">
+      <c r="G25" s="155" t="s">
         <v>74</v>
       </c>
       <c r="H25" s="24"/>
-      <c r="I25" s="157" t="s">
+      <c r="I25" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="157" t="s">
+      <c r="J25" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K25" s="26" t="s">
@@ -2719,17 +2713,17 @@
       <c r="C28" s="156"/>
       <c r="D28" s="21"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="157" t="s">
+      <c r="F28" s="155" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="157" t="s">
+      <c r="G28" s="155" t="s">
         <v>79</v>
       </c>
       <c r="H28" s="24"/>
-      <c r="I28" s="157" t="s">
+      <c r="I28" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J28" s="157" t="s">
+      <c r="J28" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K28" s="26" t="s">
@@ -2795,17 +2789,17 @@
       <c r="C32" s="156"/>
       <c r="D32" s="21"/>
       <c r="E32" s="19"/>
-      <c r="F32" s="157" t="s">
+      <c r="F32" s="155" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="157" t="s">
+      <c r="G32" s="155" t="s">
         <v>91</v>
       </c>
       <c r="H32" s="24"/>
-      <c r="I32" s="157" t="s">
+      <c r="I32" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J32" s="157" t="s">
+      <c r="J32" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K32" s="26" t="s">
@@ -2873,17 +2867,17 @@
       <c r="C36" s="156"/>
       <c r="D36" s="21"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="157" t="s">
+      <c r="F36" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="G36" s="157" t="s">
+      <c r="G36" s="155" t="s">
         <v>96</v>
       </c>
       <c r="H36" s="24"/>
-      <c r="I36" s="157" t="s">
+      <c r="I36" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J36" s="157" t="s">
+      <c r="J36" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K36" s="26" t="s">
@@ -2951,17 +2945,17 @@
       <c r="C40" s="156"/>
       <c r="D40" s="21"/>
       <c r="E40" s="19"/>
-      <c r="F40" s="157" t="s">
+      <c r="F40" s="155" t="s">
         <v>98</v>
       </c>
-      <c r="G40" s="157" t="s">
+      <c r="G40" s="155" t="s">
         <v>99</v>
       </c>
       <c r="H40" s="24"/>
-      <c r="I40" s="157" t="s">
+      <c r="I40" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J40" s="157" t="s">
+      <c r="J40" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K40" s="26" t="s">
@@ -2993,17 +2987,17 @@
       <c r="C42" s="156"/>
       <c r="D42" s="21"/>
       <c r="E42" s="19"/>
-      <c r="F42" s="157" t="s">
+      <c r="F42" s="155" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="157" t="s">
+      <c r="G42" s="155" t="s">
         <v>101</v>
       </c>
       <c r="H42" s="24"/>
-      <c r="I42" s="157" t="s">
+      <c r="I42" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J42" s="157" t="s">
+      <c r="J42" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K42" s="26" t="s">
@@ -3035,7 +3029,7 @@
       <c r="C44" s="156"/>
       <c r="D44" s="21"/>
       <c r="E44" s="19"/>
-      <c r="F44" s="157" t="s">
+      <c r="F44" s="155" t="s">
         <v>102</v>
       </c>
       <c r="G44" s="22" t="s">
@@ -3083,17 +3077,17 @@
       <c r="C46" s="156"/>
       <c r="D46" s="21"/>
       <c r="E46" s="19"/>
-      <c r="F46" s="157" t="s">
+      <c r="F46" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="157" t="s">
+      <c r="G46" s="155" t="s">
         <v>105</v>
       </c>
       <c r="H46" s="24"/>
-      <c r="I46" s="157" t="s">
+      <c r="I46" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J46" s="157" t="s">
+      <c r="J46" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K46" s="26" t="s">
@@ -3120,28 +3114,28 @@
       <c r="M47" s="26"/>
     </row>
     <row r="48" spans="1:13" ht="13.2">
-      <c r="A48" s="155" t="s">
+      <c r="A48" s="157" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="155" t="s">
+      <c r="B48" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="155" t="s">
+      <c r="C48" s="157" t="s">
         <v>107</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="19"/>
-      <c r="F48" s="157" t="s">
+      <c r="F48" s="155" t="s">
         <v>108</v>
       </c>
-      <c r="G48" s="157" t="s">
+      <c r="G48" s="155" t="s">
         <v>109</v>
       </c>
       <c r="H48" s="24"/>
-      <c r="I48" s="157" t="s">
+      <c r="I48" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J48" s="157" t="s">
+      <c r="J48" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K48" s="26" t="s">
@@ -3173,21 +3167,21 @@
       <c r="C50" s="156"/>
       <c r="D50" s="21"/>
       <c r="E50" s="19"/>
-      <c r="F50" s="157" t="s">
+      <c r="F50" s="155" t="s">
         <v>110</v>
       </c>
-      <c r="G50" s="157" t="s">
+      <c r="G50" s="155" t="s">
         <v>111</v>
       </c>
       <c r="H50" s="24"/>
-      <c r="I50" s="157" t="s">
+      <c r="I50" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J50" s="157" t="s">
+      <c r="J50" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K50" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L50" s="26"/>
       <c r="M50" s="26"/>
@@ -3204,7 +3198,7 @@
       <c r="I51" s="156"/>
       <c r="J51" s="156"/>
       <c r="K51" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L51" s="26"/>
       <c r="M51" s="26"/>
@@ -3221,34 +3215,34 @@
       <c r="I52" s="156"/>
       <c r="J52" s="156"/>
       <c r="K52" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L52" s="26"/>
       <c r="M52" s="26"/>
     </row>
     <row r="53" spans="1:13" ht="13.2">
-      <c r="A53" s="155" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="155" t="s">
+      <c r="A53" s="157" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="157" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="155" t="s">
-        <v>119</v>
+      <c r="C53" s="157" t="s">
+        <v>118</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="19"/>
-      <c r="F53" s="157" t="s">
+      <c r="F53" s="155" t="s">
+        <v>119</v>
+      </c>
+      <c r="G53" s="155" t="s">
         <v>120</v>
       </c>
-      <c r="G53" s="157" t="s">
-        <v>121</v>
-      </c>
       <c r="H53" s="24"/>
-      <c r="I53" s="157" t="s">
+      <c r="I53" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="157" t="s">
+      <c r="J53" s="155" t="s">
         <v>9</v>
       </c>
       <c r="K53" s="26" t="s">
@@ -3280,21 +3274,21 @@
       <c r="C55" s="156"/>
       <c r="D55" s="21"/>
       <c r="E55" s="19"/>
-      <c r="F55" s="157" t="s">
-        <v>117</v>
-      </c>
-      <c r="G55" s="157" t="s">
-        <v>122</v>
+      <c r="F55" s="155" t="s">
+        <v>116</v>
+      </c>
+      <c r="G55" s="155" t="s">
+        <v>121</v>
       </c>
       <c r="H55" s="24"/>
-      <c r="I55" s="157" t="s">
+      <c r="I55" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J55" s="157" t="s">
+      <c r="J55" s="155" t="s">
         <v>13</v>
       </c>
       <c r="K55" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L55" s="26"/>
       <c r="M55" s="26"/>
@@ -3311,7 +3305,7 @@
       <c r="I56" s="156"/>
       <c r="J56" s="156"/>
       <c r="K56" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L56" s="26"/>
       <c r="M56" s="26"/>
@@ -3328,23 +3322,73 @@
       <c r="I57" s="156"/>
       <c r="J57" s="156"/>
       <c r="K57" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L57" s="26"/>
       <c r="M57" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="J5:J8"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C25:C47"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="G55:G57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="C48:C52"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A25:A47"/>
+    <mergeCell ref="B25:B47"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="C2:C24"/>
+    <mergeCell ref="B2:B24"/>
+    <mergeCell ref="A2:A24"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="I50:I52"/>
+    <mergeCell ref="J50:J52"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="J55:J57"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="I55:I57"/>
     <mergeCell ref="J46:J47"/>
     <mergeCell ref="J36:J39"/>
     <mergeCell ref="J40:J41"/>
@@ -3361,66 +3405,16 @@
     <mergeCell ref="I46:I47"/>
     <mergeCell ref="I25:I27"/>
     <mergeCell ref="I28:I31"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="I50:I52"/>
-    <mergeCell ref="J50:J52"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="J55:J57"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="I55:I57"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="I13:I16"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="C2:C24"/>
-    <mergeCell ref="B2:B24"/>
-    <mergeCell ref="A2:A24"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G5:G8"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A25:A47"/>
-    <mergeCell ref="B25:B47"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="G55:G57"/>
-    <mergeCell ref="C53:C57"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G32:G35"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="C25:C47"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J8"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="J13:J16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -31518,7 +31512,7 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -31535,7 +31529,7 @@
     <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="12" width="23.44140625" customWidth="1"/>
     <col min="13" max="13" width="18.5546875" customWidth="1"/>
-    <col min="14" max="14" width="53.33203125" customWidth="1"/>
+    <col min="14" max="14" width="45.21875" customWidth="1"/>
     <col min="15" max="15" width="26.5546875" customWidth="1"/>
     <col min="16" max="16" width="25.33203125" customWidth="1"/>
     <col min="17" max="18" width="21.109375" customWidth="1"/>
@@ -31562,7 +31556,7 @@
         <v>6</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -31591,8 +31585,8 @@
       <c r="M2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="177" t="s">
-        <v>203</v>
+      <c r="N2" s="154" t="s">
+        <v>200</v>
       </c>
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
@@ -31723,7 +31717,7 @@
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
       <c r="A7" s="30"/>
-      <c r="B7" s="161" t="s">
+      <c r="B7" s="173" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="156"/>
@@ -31752,18 +31746,18 @@
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="30"/>
       <c r="B8" s="33"/>
-      <c r="C8" s="158" t="s">
+      <c r="C8" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="159"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="159"/>
-      <c r="G8" s="159"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="159"/>
-      <c r="L8" s="160"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="162"/>
+      <c r="H8" s="162"/>
+      <c r="I8" s="162"/>
+      <c r="J8" s="162"/>
+      <c r="K8" s="162"/>
+      <c r="L8" s="164"/>
       <c r="M8" s="34" t="s">
         <v>68</v>
       </c>
@@ -31802,20 +31796,20 @@
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
       <c r="A9" s="30"/>
       <c r="B9" s="33"/>
-      <c r="C9" s="162"/>
+      <c r="C9" s="168"/>
       <c r="D9" s="156"/>
       <c r="E9" s="156"/>
       <c r="F9" s="156"/>
       <c r="G9" s="156"/>
-      <c r="H9" s="163"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="167"/>
+      <c r="J9" s="172"/>
       <c r="K9" s="166" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="168"/>
+      <c r="L9" s="167"/>
       <c r="M9" s="41"/>
       <c r="N9" s="42" t="s">
         <v>97</v>
@@ -31834,25 +31828,25 @@
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
       <c r="A10" s="30"/>
       <c r="B10" s="33"/>
-      <c r="C10" s="164"/>
-      <c r="D10" s="164"/>
-      <c r="E10" s="164"/>
-      <c r="F10" s="164"/>
-      <c r="G10" s="164"/>
-      <c r="H10" s="165"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="170"/>
+      <c r="H10" s="171"/>
       <c r="I10" s="49"/>
       <c r="J10" s="50"/>
       <c r="K10" s="51"/>
       <c r="L10" s="52"/>
       <c r="M10" s="41"/>
       <c r="N10" s="53" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
       <c r="O10" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P10" s="55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q10" s="46"/>
       <c r="R10" s="46"/>
@@ -31866,37 +31860,37 @@
     <row r="11" spans="1:24" ht="17.25" customHeight="1">
       <c r="A11" s="30"/>
       <c r="B11" s="33"/>
-      <c r="C11" s="169" t="s">
+      <c r="C11" s="158" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="159"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="159"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="170"/>
-      <c r="E11" s="170"/>
-      <c r="F11" s="170"/>
-      <c r="G11" s="170"/>
-      <c r="H11" s="171"/>
-      <c r="I11" s="57" t="s">
+      <c r="J11" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="K11" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="K11" s="59" t="s">
+      <c r="L11" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="L11" s="57" t="s">
+      <c r="M11" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="M11" s="60" t="s">
+      <c r="N11" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="N11" s="60" t="s">
+      <c r="O11" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="O11" s="61" t="s">
+      <c r="P11" s="62" t="s">
         <v>130</v>
-      </c>
-      <c r="P11" s="62" t="s">
-        <v>131</v>
       </c>
       <c r="Q11" s="64"/>
       <c r="R11" s="64"/>
@@ -31914,39 +31908,39 @@
         <v>1</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E12" s="65">
         <v>1</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G12" s="67"/>
       <c r="H12" s="68"/>
       <c r="I12" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" s="69" t="s">
         <v>135</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="K12" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="K12" s="69" t="s">
+      <c r="L12" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="L12" s="69" t="s">
+      <c r="M12" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="N12" s="71">
+        <v>0</v>
+      </c>
+      <c r="O12" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="M12" s="70" t="s">
-        <v>135</v>
-      </c>
-      <c r="N12" s="71" t="s">
+      <c r="P12" s="72" t="s">
         <v>139</v>
-      </c>
-      <c r="O12" s="70" t="s">
-        <v>140</v>
-      </c>
-      <c r="P12" s="72" t="s">
-        <v>141</v>
       </c>
       <c r="Q12" s="75" t="s">
         <v>48</v>
@@ -31956,7 +31950,7 @@
         <v>questions</v>
       </c>
       <c r="S12" s="75" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T12" s="75" t="s">
         <v>48</v>
@@ -31965,7 +31959,7 @@
         <v>36</v>
       </c>
       <c r="V12" s="75" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="W12" s="76" t="s">
         <v>48</v>
@@ -31974,8 +31968,8 @@
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="161" t="s">
-        <v>145</v>
+      <c r="B13" s="173" t="s">
+        <v>143</v>
       </c>
       <c r="C13" s="156"/>
       <c r="D13" s="156"/>
@@ -32003,18 +31997,18 @@
     <row r="14" spans="1:24" ht="17.25" customHeight="1">
       <c r="A14" s="30"/>
       <c r="B14" s="33"/>
-      <c r="C14" s="158" t="s">
+      <c r="C14" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="159"/>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
-      <c r="L14" s="160"/>
+      <c r="D14" s="162"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="162"/>
+      <c r="I14" s="162"/>
+      <c r="J14" s="162"/>
+      <c r="K14" s="162"/>
+      <c r="L14" s="164"/>
       <c r="M14" s="34" t="s">
         <v>68</v>
       </c>
@@ -32053,23 +32047,23 @@
     <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="33"/>
-      <c r="C15" s="162"/>
+      <c r="C15" s="168"/>
       <c r="D15" s="156"/>
       <c r="E15" s="156"/>
       <c r="F15" s="156"/>
       <c r="G15" s="156"/>
-      <c r="H15" s="163"/>
+      <c r="H15" s="169"/>
       <c r="I15" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="J15" s="167"/>
+      <c r="J15" s="172"/>
       <c r="K15" s="166" t="s">
         <v>94</v>
       </c>
-      <c r="L15" s="168"/>
+      <c r="L15" s="167"/>
       <c r="M15" s="41"/>
       <c r="N15" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O15" s="43"/>
       <c r="P15" s="44"/>
@@ -32085,25 +32079,25 @@
     <row r="16" spans="1:24" ht="17.25" customHeight="1">
       <c r="A16" s="30"/>
       <c r="B16" s="33"/>
-      <c r="C16" s="164"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="164"/>
-      <c r="F16" s="164"/>
-      <c r="G16" s="164"/>
-      <c r="H16" s="165"/>
+      <c r="C16" s="170"/>
+      <c r="D16" s="170"/>
+      <c r="E16" s="170"/>
+      <c r="F16" s="170"/>
+      <c r="G16" s="170"/>
+      <c r="H16" s="171"/>
       <c r="I16" s="49"/>
       <c r="J16" s="50"/>
       <c r="K16" s="51"/>
       <c r="L16" s="52"/>
       <c r="M16" s="41"/>
       <c r="N16" s="53" t="s">
-        <v>148</v>
+        <v>201</v>
       </c>
       <c r="O16" s="54" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P16" s="55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q16" s="46"/>
       <c r="R16" s="46"/>
@@ -32117,37 +32111,37 @@
     <row r="17" spans="1:24" ht="17.25" customHeight="1">
       <c r="A17" s="30"/>
       <c r="B17" s="33"/>
-      <c r="C17" s="173" t="s">
+      <c r="C17" s="165" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="159"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="159"/>
+      <c r="G17" s="159"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="170"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="170"/>
-      <c r="H17" s="171"/>
-      <c r="I17" s="57" t="s">
+      <c r="J17" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="J17" s="58" t="s">
+      <c r="K17" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="K17" s="59" t="s">
+      <c r="L17" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="L17" s="57" t="s">
+      <c r="M17" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="M17" s="60" t="s">
-        <v>128</v>
-      </c>
       <c r="N17" s="60" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="O17" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P17" s="62" t="s">
         <v>130</v>
-      </c>
-      <c r="P17" s="62" t="s">
-        <v>131</v>
       </c>
       <c r="Q17" s="64"/>
       <c r="R17" s="64"/>
@@ -32165,39 +32159,39 @@
         <v>2</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" s="65">
         <v>1</v>
       </c>
       <c r="F18" s="66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G18" s="67"/>
       <c r="H18" s="68"/>
       <c r="I18" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="J18" s="69" t="s">
+        <v>150</v>
+      </c>
+      <c r="K18" s="69" t="s">
+        <v>151</v>
+      </c>
+      <c r="L18" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="J18" s="69" t="s">
+      <c r="M18" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="N18" s="71">
+        <v>0</v>
+      </c>
+      <c r="O18" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="K18" s="69" t="s">
+      <c r="P18" s="70" t="s">
         <v>154</v>
-      </c>
-      <c r="L18" s="69" t="s">
-        <v>155</v>
-      </c>
-      <c r="M18" s="70" t="s">
-        <v>152</v>
-      </c>
-      <c r="N18" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="O18" s="70" t="s">
-        <v>156</v>
-      </c>
-      <c r="P18" s="70" t="s">
-        <v>157</v>
       </c>
       <c r="Q18" s="75" t="s">
         <v>48</v>
@@ -32207,7 +32201,7 @@
         <v>options</v>
       </c>
       <c r="S18" s="75" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T18" s="75" t="s">
         <v>48</v>
@@ -32216,7 +32210,7 @@
         <v>36</v>
       </c>
       <c r="V18" s="75" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="W18" s="76" t="s">
         <v>48</v>
@@ -32225,23 +32219,23 @@
     </row>
     <row r="19" spans="1:24" ht="17.25" customHeight="1">
       <c r="A19" s="80"/>
-      <c r="B19" s="172" t="s">
-        <v>159</v>
-      </c>
-      <c r="C19" s="159"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="159"/>
-      <c r="O19" s="159"/>
-      <c r="P19" s="159"/>
+      <c r="B19" s="161" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="162"/>
+      <c r="D19" s="162"/>
+      <c r="E19" s="162"/>
+      <c r="F19" s="162"/>
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162"/>
+      <c r="J19" s="162"/>
+      <c r="K19" s="162"/>
+      <c r="L19" s="162"/>
+      <c r="M19" s="162"/>
+      <c r="N19" s="162"/>
+      <c r="O19" s="162"/>
+      <c r="P19" s="162"/>
       <c r="Q19" s="91"/>
       <c r="R19" s="91"/>
       <c r="S19" s="91"/>
@@ -32254,18 +32248,18 @@
     <row r="20" spans="1:24" ht="36">
       <c r="A20" s="80"/>
       <c r="B20" s="85"/>
-      <c r="C20" s="158" t="s">
+      <c r="C20" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="159"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="159"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="159"/>
-      <c r="I20" s="159"/>
-      <c r="J20" s="159"/>
-      <c r="K20" s="159"/>
-      <c r="L20" s="160"/>
+      <c r="D20" s="162"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="162"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162"/>
+      <c r="J20" s="162"/>
+      <c r="K20" s="162"/>
+      <c r="L20" s="164"/>
       <c r="M20" s="86" t="s">
         <v>68</v>
       </c>
@@ -32304,23 +32298,23 @@
     <row r="21" spans="1:24" ht="18">
       <c r="A21" s="80"/>
       <c r="B21" s="85"/>
-      <c r="C21" s="162"/>
+      <c r="C21" s="168"/>
       <c r="D21" s="156"/>
       <c r="E21" s="156"/>
       <c r="F21" s="156"/>
       <c r="G21" s="156"/>
-      <c r="H21" s="163"/>
+      <c r="H21" s="169"/>
       <c r="I21" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="J21" s="167"/>
+      <c r="J21" s="172"/>
       <c r="K21" s="166" t="s">
         <v>94</v>
       </c>
-      <c r="L21" s="168"/>
+      <c r="L21" s="167"/>
       <c r="M21" s="94"/>
       <c r="N21" s="95" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O21" s="96"/>
       <c r="P21" s="45"/>
@@ -32336,25 +32330,25 @@
     <row r="22" spans="1:24" ht="17.25" customHeight="1">
       <c r="A22" s="80"/>
       <c r="B22" s="85"/>
-      <c r="C22" s="164"/>
-      <c r="D22" s="164"/>
-      <c r="E22" s="164"/>
-      <c r="F22" s="164"/>
-      <c r="G22" s="164"/>
-      <c r="H22" s="165"/>
+      <c r="C22" s="170"/>
+      <c r="D22" s="170"/>
+      <c r="E22" s="170"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="170"/>
+      <c r="H22" s="171"/>
       <c r="I22" s="49"/>
       <c r="J22" s="50"/>
       <c r="K22" s="51"/>
       <c r="L22" s="52"/>
       <c r="M22" s="94"/>
-      <c r="N22" s="102" t="s">
-        <v>162</v>
-      </c>
-      <c r="O22" s="103" t="s">
-        <v>163</v>
+      <c r="N22" s="104" t="s">
+        <v>159</v>
+      </c>
+      <c r="O22" s="102" t="s">
+        <v>160</v>
       </c>
       <c r="P22" s="56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q22" s="89"/>
       <c r="R22" s="89"/>
@@ -32368,43 +32362,43 @@
     <row r="23" spans="1:24" ht="18">
       <c r="A23" s="80"/>
       <c r="B23" s="85"/>
-      <c r="C23" s="169" t="s">
+      <c r="C23" s="158" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="105" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="170"/>
-      <c r="E23" s="170"/>
-      <c r="F23" s="170"/>
-      <c r="G23" s="170"/>
-      <c r="H23" s="171"/>
-      <c r="I23" s="106" t="s">
+      <c r="J23" s="106" t="s">
         <v>124</v>
       </c>
-      <c r="J23" s="107" t="s">
+      <c r="K23" s="107" t="s">
         <v>125</v>
       </c>
-      <c r="K23" s="108" t="s">
+      <c r="L23" s="105" t="s">
         <v>126</v>
       </c>
-      <c r="L23" s="106" t="s">
+      <c r="M23" s="109" t="s">
         <v>127</v>
       </c>
-      <c r="M23" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="N23" s="110" t="s">
-        <v>167</v>
-      </c>
-      <c r="O23" s="112" t="s">
-        <v>130</v>
+      <c r="N23" s="109" t="s">
+        <v>164</v>
+      </c>
+      <c r="O23" s="111" t="s">
+        <v>129</v>
       </c>
       <c r="P23" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q23" s="114"/>
-      <c r="R23" s="114"/>
-      <c r="S23" s="114"/>
-      <c r="T23" s="114"/>
-      <c r="U23" s="114"/>
+        <v>131</v>
+      </c>
+      <c r="Q23" s="113"/>
+      <c r="R23" s="113"/>
+      <c r="S23" s="113"/>
+      <c r="T23" s="113"/>
+      <c r="U23" s="113"/>
       <c r="V23" s="90"/>
       <c r="W23" s="90"/>
       <c r="X23" s="98"/>
@@ -32412,36 +32406,36 @@
     <row r="24" spans="1:24" ht="69" customHeight="1">
       <c r="A24" s="80"/>
       <c r="B24" s="85"/>
-      <c r="C24" s="117">
+      <c r="C24" s="116">
         <v>5</v>
       </c>
-      <c r="D24" s="119" t="s">
+      <c r="D24" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" s="116">
+        <v>1</v>
+      </c>
+      <c r="F24" s="120" t="s">
+        <v>166</v>
+      </c>
+      <c r="G24" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="117">
-        <v>1</v>
-      </c>
-      <c r="F24" s="121" t="s">
+      <c r="H24" s="124" t="s">
+        <v>148</v>
+      </c>
+      <c r="I24" s="125" t="s">
+        <v>167</v>
+      </c>
+      <c r="J24" s="125"/>
+      <c r="K24" s="125" t="s">
+        <v>168</v>
+      </c>
+      <c r="L24" s="125"/>
+      <c r="M24" s="126" t="s">
         <v>169</v>
       </c>
-      <c r="G24" s="123" t="s">
-        <v>134</v>
-      </c>
-      <c r="H24" s="125" t="s">
-        <v>151</v>
-      </c>
-      <c r="I24" s="126" t="s">
-        <v>170</v>
-      </c>
-      <c r="J24" s="126"/>
-      <c r="K24" s="126" t="s">
-        <v>171</v>
-      </c>
-      <c r="L24" s="126"/>
-      <c r="M24" s="127" t="s">
-        <v>172</v>
-      </c>
-      <c r="N24" s="129" t="str">
+      <c r="N24" s="128" t="str">
         <f>CONCATENATE("""",Questions!$F$2,"""", ",","""",Questions!$K$3,"""")</f>
         <v>"4b44037b-a78d-4a64-bd07-617f8111a9b3","No"</v>
       </c>
@@ -32453,65 +32447,65 @@
         <f t="shared" ref="P24:P25" si="0">CONCATENATE("""","DEBUG","""",",","""",H24,"""")</f>
         <v>"DEBUG","options"</v>
       </c>
-      <c r="Q24" s="132" t="s">
+      <c r="Q24" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="R24" s="132" t="str">
+      <c r="R24" s="131" t="str">
         <f t="shared" ref="R24:R25" si="1">SUBSTITUTE(TRIM(F24&amp;" "&amp;G24&amp;" "&amp;H24)," ","-")</f>
         <v>form-questions-options</v>
       </c>
-      <c r="S24" s="132" t="s">
-        <v>179</v>
-      </c>
-      <c r="T24" s="134" t="str">
+      <c r="S24" s="131" t="s">
+        <v>176</v>
+      </c>
+      <c r="T24" s="133" t="str">
         <f t="shared" ref="T24:T25" si="2">IF(N24="COMPLETE","false","true")</f>
         <v>true</v>
       </c>
-      <c r="U24" s="134" t="str">
+      <c r="U24" s="133" t="str">
         <f t="shared" ref="U24:U25" si="3">IF(M24="COMPLETE","false","true")</f>
         <v>true</v>
       </c>
-      <c r="V24" s="132" t="s">
-        <v>180</v>
-      </c>
-      <c r="W24" s="132" t="s">
+      <c r="V24" s="131" t="s">
+        <v>177</v>
+      </c>
+      <c r="W24" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="X24" s="136"/>
+      <c r="X24" s="135"/>
     </row>
     <row r="25" spans="1:24" ht="67.5" customHeight="1">
       <c r="A25" s="80"/>
       <c r="B25" s="85"/>
-      <c r="C25" s="117">
+      <c r="C25" s="116">
         <v>5</v>
       </c>
-      <c r="D25" s="119" t="s">
+      <c r="D25" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="116">
+        <v>2</v>
+      </c>
+      <c r="F25" s="120" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="E25" s="117">
-        <v>2</v>
-      </c>
-      <c r="F25" s="121" t="s">
-        <v>169</v>
-      </c>
-      <c r="G25" s="123" t="s">
-        <v>134</v>
-      </c>
-      <c r="H25" s="125" t="s">
-        <v>151</v>
-      </c>
-      <c r="I25" s="126" t="s">
-        <v>170</v>
-      </c>
-      <c r="J25" s="126"/>
-      <c r="K25" s="126" t="s">
-        <v>171</v>
-      </c>
-      <c r="L25" s="126"/>
-      <c r="M25" s="127" t="s">
-        <v>181</v>
-      </c>
-      <c r="N25" s="129" t="str">
+      <c r="H25" s="124" t="s">
+        <v>148</v>
+      </c>
+      <c r="I25" s="125" t="s">
+        <v>167</v>
+      </c>
+      <c r="J25" s="125"/>
+      <c r="K25" s="125" t="s">
+        <v>168</v>
+      </c>
+      <c r="L25" s="125"/>
+      <c r="M25" s="126" t="s">
+        <v>178</v>
+      </c>
+      <c r="N25" s="128" t="str">
         <f>CONCATENATE("""",Questions!$F$25,"""", ",","""",Questions!$K$26,"""")</f>
         <v>"4e5a67c4-b02e-45dd-be94-d675b622f22a","No"</v>
       </c>
@@ -32523,276 +32517,268 @@
         <f t="shared" si="0"/>
         <v>"DEBUG","options"</v>
       </c>
-      <c r="Q25" s="132" t="s">
+      <c r="Q25" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="R25" s="132" t="str">
+      <c r="R25" s="131" t="str">
         <f t="shared" si="1"/>
         <v>form-questions-options</v>
       </c>
-      <c r="S25" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="T25" s="134" t="str">
+      <c r="S25" s="131" t="s">
+        <v>183</v>
+      </c>
+      <c r="T25" s="133" t="str">
         <f t="shared" si="2"/>
         <v>true</v>
       </c>
-      <c r="U25" s="134" t="str">
+      <c r="U25" s="133" t="str">
         <f t="shared" si="3"/>
         <v>true</v>
       </c>
-      <c r="V25" s="132" t="s">
-        <v>180</v>
-      </c>
-      <c r="W25" s="132" t="s">
+      <c r="V25" s="131" t="s">
+        <v>177</v>
+      </c>
+      <c r="W25" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="X25" s="136"/>
+      <c r="X25" s="135"/>
     </row>
     <row r="26" spans="1:24" ht="14.4">
-      <c r="A26" s="138"/>
-      <c r="B26" s="138"/>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="141"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="138"/>
-      <c r="I26" s="142"/>
-      <c r="J26" s="142"/>
-      <c r="K26" s="142"/>
-      <c r="L26" s="142"/>
-      <c r="M26" s="143"/>
-      <c r="N26" s="144"/>
-      <c r="O26" s="140"/>
-      <c r="P26" s="145"/>
-      <c r="Q26" s="146"/>
-      <c r="R26" s="146"/>
-      <c r="S26" s="147"/>
-      <c r="T26" s="147"/>
-      <c r="U26" s="148"/>
-      <c r="V26" s="148"/>
-      <c r="W26" s="148"/>
-      <c r="X26" s="148"/>
+      <c r="A26" s="137"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="137"/>
+      <c r="H26" s="137"/>
+      <c r="I26" s="141"/>
+      <c r="J26" s="141"/>
+      <c r="K26" s="141"/>
+      <c r="L26" s="141"/>
+      <c r="M26" s="142"/>
+      <c r="N26" s="143"/>
+      <c r="O26" s="139"/>
+      <c r="P26" s="144"/>
+      <c r="Q26" s="145"/>
+      <c r="R26" s="145"/>
+      <c r="S26" s="146"/>
+      <c r="T26" s="146"/>
+      <c r="U26" s="147"/>
+      <c r="V26" s="147"/>
+      <c r="W26" s="147"/>
+      <c r="X26" s="147"/>
     </row>
     <row r="27" spans="1:24" ht="14.4">
-      <c r="A27" s="138"/>
-      <c r="B27" s="138"/>
-      <c r="C27" s="140"/>
-      <c r="D27" s="140"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="141"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="142"/>
-      <c r="J27" s="142"/>
-      <c r="K27" s="142"/>
-      <c r="L27" s="142"/>
-      <c r="M27" s="143"/>
-      <c r="N27" s="144"/>
-      <c r="O27" s="140"/>
-      <c r="P27" s="145"/>
-      <c r="Q27" s="146"/>
-      <c r="R27" s="146"/>
-      <c r="S27" s="147"/>
-      <c r="T27" s="147"/>
-      <c r="U27" s="148"/>
-      <c r="V27" s="148"/>
-      <c r="W27" s="148"/>
-      <c r="X27" s="148"/>
+      <c r="A27" s="137"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="139"/>
+      <c r="D27" s="139"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="141"/>
+      <c r="J27" s="141"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="141"/>
+      <c r="M27" s="142"/>
+      <c r="N27" s="143"/>
+      <c r="O27" s="139"/>
+      <c r="P27" s="144"/>
+      <c r="Q27" s="145"/>
+      <c r="R27" s="145"/>
+      <c r="S27" s="146"/>
+      <c r="T27" s="146"/>
+      <c r="U27" s="147"/>
+      <c r="V27" s="147"/>
+      <c r="W27" s="147"/>
+      <c r="X27" s="147"/>
     </row>
     <row r="28" spans="1:24" ht="14.4">
-      <c r="A28" s="138"/>
-      <c r="B28" s="138"/>
-      <c r="C28" s="140"/>
-      <c r="D28" s="140"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="141"/>
-      <c r="G28" s="138"/>
-      <c r="H28" s="138"/>
-      <c r="I28" s="142"/>
-      <c r="J28" s="142"/>
-      <c r="K28" s="142"/>
-      <c r="L28" s="142"/>
-      <c r="M28" s="143"/>
-      <c r="N28" s="144"/>
-      <c r="O28" s="140"/>
-      <c r="P28" s="145"/>
-      <c r="Q28" s="146"/>
-      <c r="R28" s="146"/>
-      <c r="S28" s="147"/>
-      <c r="T28" s="147"/>
-      <c r="U28" s="148"/>
-      <c r="V28" s="148"/>
-      <c r="W28" s="148"/>
-      <c r="X28" s="148"/>
+      <c r="A28" s="137"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="137"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="141"/>
+      <c r="K28" s="141"/>
+      <c r="L28" s="141"/>
+      <c r="M28" s="142"/>
+      <c r="N28" s="143"/>
+      <c r="O28" s="139"/>
+      <c r="P28" s="144"/>
+      <c r="Q28" s="145"/>
+      <c r="R28" s="145"/>
+      <c r="S28" s="146"/>
+      <c r="T28" s="146"/>
+      <c r="U28" s="147"/>
+      <c r="V28" s="147"/>
+      <c r="W28" s="147"/>
+      <c r="X28" s="147"/>
     </row>
     <row r="29" spans="1:24" ht="14.4">
-      <c r="A29" s="138"/>
-      <c r="B29" s="138"/>
-      <c r="C29" s="140"/>
-      <c r="D29" s="140"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="141"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="138"/>
-      <c r="I29" s="142"/>
-      <c r="J29" s="142"/>
-      <c r="K29" s="142"/>
-      <c r="L29" s="142"/>
-      <c r="M29" s="143"/>
-      <c r="N29" s="144"/>
-      <c r="O29" s="140"/>
-      <c r="P29" s="145"/>
-      <c r="Q29" s="146"/>
-      <c r="R29" s="146"/>
-      <c r="S29" s="147"/>
-      <c r="T29" s="147"/>
-      <c r="U29" s="148"/>
-      <c r="V29" s="148"/>
-      <c r="W29" s="148"/>
-      <c r="X29" s="148"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="137"/>
+      <c r="H29" s="137"/>
+      <c r="I29" s="141"/>
+      <c r="J29" s="141"/>
+      <c r="K29" s="141"/>
+      <c r="L29" s="141"/>
+      <c r="M29" s="142"/>
+      <c r="N29" s="143"/>
+      <c r="O29" s="139"/>
+      <c r="P29" s="144"/>
+      <c r="Q29" s="145"/>
+      <c r="R29" s="145"/>
+      <c r="S29" s="146"/>
+      <c r="T29" s="146"/>
+      <c r="U29" s="147"/>
+      <c r="V29" s="147"/>
+      <c r="W29" s="147"/>
+      <c r="X29" s="147"/>
     </row>
     <row r="30" spans="1:24" ht="14.4">
-      <c r="A30" s="138"/>
-      <c r="B30" s="138"/>
-      <c r="C30" s="140"/>
-      <c r="D30" s="140"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="141"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="138"/>
-      <c r="I30" s="142"/>
-      <c r="J30" s="142"/>
-      <c r="K30" s="142"/>
-      <c r="L30" s="142"/>
-      <c r="M30" s="143"/>
-      <c r="N30" s="144"/>
-      <c r="O30" s="140"/>
-      <c r="P30" s="145"/>
-      <c r="Q30" s="146"/>
-      <c r="R30" s="146"/>
-      <c r="S30" s="147"/>
-      <c r="T30" s="147"/>
-      <c r="U30" s="148"/>
-      <c r="V30" s="148"/>
-      <c r="W30" s="148"/>
-      <c r="X30" s="148"/>
+      <c r="A30" s="137"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="137"/>
+      <c r="I30" s="141"/>
+      <c r="J30" s="141"/>
+      <c r="K30" s="141"/>
+      <c r="L30" s="141"/>
+      <c r="M30" s="142"/>
+      <c r="N30" s="143"/>
+      <c r="O30" s="139"/>
+      <c r="P30" s="144"/>
+      <c r="Q30" s="145"/>
+      <c r="R30" s="145"/>
+      <c r="S30" s="146"/>
+      <c r="T30" s="146"/>
+      <c r="U30" s="147"/>
+      <c r="V30" s="147"/>
+      <c r="W30" s="147"/>
+      <c r="X30" s="147"/>
     </row>
     <row r="31" spans="1:24" ht="14.4">
-      <c r="A31" s="138"/>
-      <c r="B31" s="138"/>
-      <c r="C31" s="140"/>
-      <c r="D31" s="140"/>
-      <c r="E31" s="140"/>
-      <c r="F31" s="141"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="138"/>
-      <c r="I31" s="142"/>
-      <c r="J31" s="142"/>
-      <c r="K31" s="142"/>
-      <c r="L31" s="142"/>
-      <c r="M31" s="143"/>
-      <c r="N31" s="144"/>
-      <c r="O31" s="140"/>
-      <c r="P31" s="145"/>
-      <c r="Q31" s="146"/>
-      <c r="R31" s="146"/>
-      <c r="S31" s="147"/>
-      <c r="T31" s="147"/>
-      <c r="U31" s="148"/>
-      <c r="V31" s="148"/>
-      <c r="W31" s="148"/>
-      <c r="X31" s="148"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="137"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="139"/>
+      <c r="E31" s="139"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="137"/>
+      <c r="I31" s="141"/>
+      <c r="J31" s="141"/>
+      <c r="K31" s="141"/>
+      <c r="L31" s="141"/>
+      <c r="M31" s="142"/>
+      <c r="N31" s="143"/>
+      <c r="O31" s="139"/>
+      <c r="P31" s="144"/>
+      <c r="Q31" s="145"/>
+      <c r="R31" s="145"/>
+      <c r="S31" s="146"/>
+      <c r="T31" s="146"/>
+      <c r="U31" s="147"/>
+      <c r="V31" s="147"/>
+      <c r="W31" s="147"/>
+      <c r="X31" s="147"/>
     </row>
     <row r="32" spans="1:24" ht="14.4">
-      <c r="A32" s="138"/>
-      <c r="B32" s="138"/>
-      <c r="C32" s="140"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="140"/>
-      <c r="F32" s="141"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="138"/>
-      <c r="I32" s="142"/>
-      <c r="J32" s="142"/>
-      <c r="K32" s="142"/>
-      <c r="L32" s="142"/>
-      <c r="M32" s="143"/>
-      <c r="N32" s="144"/>
-      <c r="O32" s="140"/>
-      <c r="P32" s="145"/>
-      <c r="Q32" s="146"/>
-      <c r="R32" s="146"/>
-      <c r="S32" s="147"/>
-      <c r="T32" s="147"/>
-      <c r="U32" s="148"/>
-      <c r="V32" s="148"/>
-      <c r="W32" s="148"/>
-      <c r="X32" s="148"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="137"/>
+      <c r="C32" s="139"/>
+      <c r="D32" s="139"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="137"/>
+      <c r="H32" s="137"/>
+      <c r="I32" s="141"/>
+      <c r="J32" s="141"/>
+      <c r="K32" s="141"/>
+      <c r="L32" s="141"/>
+      <c r="M32" s="142"/>
+      <c r="N32" s="143"/>
+      <c r="O32" s="139"/>
+      <c r="P32" s="144"/>
+      <c r="Q32" s="145"/>
+      <c r="R32" s="145"/>
+      <c r="S32" s="146"/>
+      <c r="T32" s="146"/>
+      <c r="U32" s="147"/>
+      <c r="V32" s="147"/>
+      <c r="W32" s="147"/>
+      <c r="X32" s="147"/>
     </row>
     <row r="33" spans="1:24" ht="14.4">
-      <c r="A33" s="138"/>
-      <c r="B33" s="138"/>
-      <c r="C33" s="140"/>
-      <c r="D33" s="140"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="141"/>
-      <c r="G33" s="138"/>
-      <c r="H33" s="138"/>
-      <c r="I33" s="142"/>
-      <c r="J33" s="142"/>
-      <c r="K33" s="142"/>
-      <c r="L33" s="142"/>
-      <c r="M33" s="143"/>
-      <c r="N33" s="144"/>
-      <c r="O33" s="140"/>
-      <c r="P33" s="145"/>
-      <c r="Q33" s="146"/>
-      <c r="R33" s="146"/>
-      <c r="S33" s="147"/>
-      <c r="T33" s="147"/>
-      <c r="U33" s="148"/>
-      <c r="V33" s="148"/>
-      <c r="W33" s="148"/>
-      <c r="X33" s="148"/>
+      <c r="A33" s="137"/>
+      <c r="B33" s="137"/>
+      <c r="C33" s="139"/>
+      <c r="D33" s="139"/>
+      <c r="E33" s="139"/>
+      <c r="F33" s="140"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="137"/>
+      <c r="I33" s="141"/>
+      <c r="J33" s="141"/>
+      <c r="K33" s="141"/>
+      <c r="L33" s="141"/>
+      <c r="M33" s="142"/>
+      <c r="N33" s="143"/>
+      <c r="O33" s="139"/>
+      <c r="P33" s="144"/>
+      <c r="Q33" s="145"/>
+      <c r="R33" s="145"/>
+      <c r="S33" s="146"/>
+      <c r="T33" s="146"/>
+      <c r="U33" s="147"/>
+      <c r="V33" s="147"/>
+      <c r="W33" s="147"/>
+      <c r="X33" s="147"/>
     </row>
     <row r="34" spans="1:24" ht="14.4">
-      <c r="A34" s="138"/>
-      <c r="B34" s="138"/>
-      <c r="C34" s="140"/>
-      <c r="D34" s="140"/>
-      <c r="E34" s="140"/>
-      <c r="F34" s="141"/>
-      <c r="G34" s="138"/>
-      <c r="H34" s="138"/>
-      <c r="I34" s="142"/>
-      <c r="J34" s="142"/>
-      <c r="K34" s="142"/>
-      <c r="L34" s="142"/>
-      <c r="M34" s="143"/>
-      <c r="N34" s="144"/>
-      <c r="O34" s="140"/>
-      <c r="P34" s="145"/>
-      <c r="Q34" s="146"/>
-      <c r="R34" s="146"/>
-      <c r="S34" s="147"/>
-      <c r="T34" s="147"/>
-      <c r="U34" s="148"/>
-      <c r="V34" s="148"/>
-      <c r="W34" s="148"/>
-      <c r="X34" s="148"/>
+      <c r="A34" s="137"/>
+      <c r="B34" s="137"/>
+      <c r="C34" s="139"/>
+      <c r="D34" s="139"/>
+      <c r="E34" s="139"/>
+      <c r="F34" s="140"/>
+      <c r="G34" s="137"/>
+      <c r="H34" s="137"/>
+      <c r="I34" s="141"/>
+      <c r="J34" s="141"/>
+      <c r="K34" s="141"/>
+      <c r="L34" s="141"/>
+      <c r="M34" s="142"/>
+      <c r="N34" s="143"/>
+      <c r="O34" s="139"/>
+      <c r="P34" s="144"/>
+      <c r="Q34" s="145"/>
+      <c r="R34" s="145"/>
+      <c r="S34" s="146"/>
+      <c r="T34" s="146"/>
+      <c r="U34" s="147"/>
+      <c r="V34" s="147"/>
+      <c r="W34" s="147"/>
+      <c r="X34" s="147"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="B19:P19"/>
-    <mergeCell ref="C20:L20"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C21:H22"/>
-    <mergeCell ref="I21:J21"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="B7:P7"/>
     <mergeCell ref="C15:H16"/>
@@ -32803,6 +32789,14 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="B19:P19"/>
+    <mergeCell ref="C20:L20"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C21:H22"/>
+    <mergeCell ref="I21:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -32904,7 +32898,7 @@
         <v>21</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
@@ -33014,24 +33008,24 @@
     </row>
     <row r="5" spans="1:37" ht="16.5" customHeight="1">
       <c r="A5" s="80"/>
-      <c r="B5" s="172" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="159"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="159"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
+      <c r="B5" s="161" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="162"/>
+      <c r="H5" s="162"/>
+      <c r="I5" s="162"/>
+      <c r="J5" s="162"/>
+      <c r="K5" s="162"/>
+      <c r="L5" s="162"/>
+      <c r="M5" s="162"/>
+      <c r="N5" s="162"/>
+      <c r="O5" s="162"/>
+      <c r="P5" s="162"/>
+      <c r="Q5" s="162"/>
       <c r="R5" s="81"/>
       <c r="S5" s="82"/>
       <c r="T5" s="82"/>
@@ -33056,18 +33050,18 @@
     <row r="6" spans="1:37" ht="18">
       <c r="A6" s="80"/>
       <c r="B6" s="85"/>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
-      <c r="J6" s="159"/>
-      <c r="K6" s="159"/>
-      <c r="L6" s="160"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="162"/>
+      <c r="H6" s="162"/>
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+      <c r="L6" s="164"/>
       <c r="M6" s="86" t="s">
         <v>68</v>
       </c>
@@ -33117,23 +33111,23 @@
     <row r="7" spans="1:37" ht="18">
       <c r="A7" s="80"/>
       <c r="B7" s="85"/>
-      <c r="C7" s="162"/>
+      <c r="C7" s="168"/>
       <c r="D7" s="156"/>
       <c r="E7" s="156"/>
       <c r="F7" s="156"/>
       <c r="G7" s="156"/>
-      <c r="H7" s="163"/>
+      <c r="H7" s="169"/>
       <c r="I7" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="167"/>
+      <c r="J7" s="172"/>
       <c r="K7" s="166" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="168"/>
+      <c r="L7" s="167"/>
       <c r="M7" s="94"/>
       <c r="N7" s="174" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O7" s="175"/>
       <c r="P7" s="96"/>
@@ -33162,28 +33156,28 @@
     <row r="8" spans="1:37" ht="18.75" customHeight="1">
       <c r="A8" s="80"/>
       <c r="B8" s="85"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="164"/>
-      <c r="H8" s="165"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="170"/>
+      <c r="F8" s="170"/>
+      <c r="G8" s="170"/>
+      <c r="H8" s="171"/>
       <c r="I8" s="99"/>
       <c r="J8" s="100"/>
       <c r="K8" s="101"/>
-      <c r="L8" s="104"/>
+      <c r="L8" s="103"/>
       <c r="M8" s="94"/>
-      <c r="N8" s="105" t="s">
-        <v>164</v>
-      </c>
-      <c r="O8" s="105" t="s">
-        <v>165</v>
-      </c>
-      <c r="P8" s="103" t="s">
-        <v>166</v>
+      <c r="N8" s="104" t="s">
+        <v>161</v>
+      </c>
+      <c r="O8" s="104" t="s">
+        <v>162</v>
+      </c>
+      <c r="P8" s="102" t="s">
+        <v>163</v>
       </c>
       <c r="Q8" s="56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R8" s="97"/>
       <c r="S8" s="89"/>
@@ -33208,48 +33202,48 @@
     </row>
     <row r="9" spans="1:37" ht="18">
       <c r="A9" s="3"/>
-      <c r="B9" s="109"/>
-      <c r="C9" s="169" t="s">
+      <c r="B9" s="108"/>
+      <c r="C9" s="158" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="159"/>
+      <c r="E9" s="159"/>
+      <c r="F9" s="159"/>
+      <c r="G9" s="159"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="171"/>
-      <c r="I9" s="111" t="s">
+      <c r="J9" s="112" t="s">
         <v>124</v>
       </c>
-      <c r="J9" s="113" t="s">
+      <c r="K9" s="114" t="s">
         <v>125</v>
       </c>
-      <c r="K9" s="115" t="s">
+      <c r="L9" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="L9" s="111" t="s">
+      <c r="M9" s="115" t="s">
         <v>127</v>
       </c>
-      <c r="M9" s="116" t="s">
-        <v>128</v>
-      </c>
-      <c r="N9" s="116" t="s">
-        <v>167</v>
-      </c>
-      <c r="O9" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="P9" s="120" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q9" s="122" t="s">
-        <v>132</v>
-      </c>
-      <c r="R9" s="124"/>
-      <c r="S9" s="114"/>
-      <c r="T9" s="114"/>
-      <c r="U9" s="114"/>
-      <c r="V9" s="114"/>
-      <c r="W9" s="114"/>
+      <c r="N9" s="115" t="s">
+        <v>164</v>
+      </c>
+      <c r="O9" s="117" t="s">
+        <v>165</v>
+      </c>
+      <c r="P9" s="119" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q9" s="121" t="s">
+        <v>131</v>
+      </c>
+      <c r="R9" s="123"/>
+      <c r="S9" s="113"/>
+      <c r="T9" s="113"/>
+      <c r="U9" s="113"/>
+      <c r="V9" s="113"/>
+      <c r="W9" s="113"/>
       <c r="X9" s="90"/>
       <c r="Y9" s="90"/>
       <c r="Z9" s="90"/>
@@ -33268,62 +33262,62 @@
     <row r="10" spans="1:37" ht="19.5" customHeight="1">
       <c r="A10" s="80"/>
       <c r="B10" s="85"/>
-      <c r="C10" s="119">
+      <c r="C10" s="118">
         <v>1</v>
       </c>
-      <c r="D10" s="119" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" s="119">
+      <c r="D10" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="118">
         <v>1</v>
       </c>
-      <c r="F10" s="121" t="s">
-        <v>169</v>
-      </c>
-      <c r="G10" s="123" t="s">
+      <c r="F10" s="120" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="122" t="s">
+        <v>170</v>
+      </c>
+      <c r="H10" s="122"/>
+      <c r="I10" s="125" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" s="127" t="s">
+        <v>172</v>
+      </c>
+      <c r="K10" s="125" t="s">
         <v>173</v>
       </c>
-      <c r="H10" s="123"/>
-      <c r="I10" s="126" t="s">
+      <c r="L10" s="125" t="s">
         <v>174</v>
       </c>
-      <c r="J10" s="128" t="s">
-        <v>175</v>
-      </c>
-      <c r="K10" s="126" t="s">
-        <v>176</v>
-      </c>
-      <c r="L10" s="126" t="s">
-        <v>177</v>
-      </c>
-      <c r="M10" s="130" t="str">
+      <c r="M10" s="129" t="str">
         <f t="shared" ref="M10:M11" si="0">I10</f>
         <v>Form\'s description cannot be null</v>
       </c>
-      <c r="N10" s="131" t="s">
-        <v>178</v>
-      </c>
-      <c r="O10" s="131"/>
+      <c r="N10" s="130" t="s">
+        <v>175</v>
+      </c>
+      <c r="O10" s="130"/>
       <c r="P10" s="74" t="str">
         <f t="shared" ref="P10:P11" si="1">CONCATENATE("""",CONCATENATE("form[","$form.getId()","]"),"""",",","""",SUBSTITUTE(TRIM(F10&amp;" "&amp;G10&amp;" "&amp;H10)," ","."),"""",",","""",$I$7,"""",",","""",CONCATENATE(C10,D10,E10)," [",SUBSTITUTE(TRIM(F10&amp;" "&amp;G10&amp;" "&amp;H10)," ","."),"] - ",I10,"""",",","""",I10,"""",",","""",J10,"""",",","""", $K$7,"""",",","""",CONCATENATE(C10,D10,E10)," [",SUBSTITUTE(TRIM(F10&amp;" "&amp;G10&amp;" "&amp;H10)," ","."),"] - ",K10,"""",",","""",K10,"""",",","""",L10,"""",",","$form.getDescription()",",","$form.getId()")</f>
         <v>"form[$form.getId()]","form.description","en","1.1 [form.description] - Form\'s description cannot be null","Form\'s description cannot be null","A name with some value different than null","es","1.1 [form.description] - La descripción de la forma no pude ser nulo","La descripción de la forma no pude ser nulo","Una descripción con algún valor diferente de nulo",$form.getDescription(),$form.getId()</v>
       </c>
-      <c r="Q10" s="133" t="str">
+      <c r="Q10" s="132" t="str">
         <f t="shared" ref="Q10:Q11" si="2">CONCATENATE("""","ERROR","""",",","""",I10,"""")</f>
         <v>"ERROR","Form\'s description cannot be null"</v>
       </c>
-      <c r="R10" s="135"/>
-      <c r="S10" s="134" t="s">
+      <c r="R10" s="134"/>
+      <c r="S10" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="T10" s="137" t="str">
+      <c r="T10" s="136" t="str">
         <f t="shared" ref="T10:T11" si="3">SUBSTITUTE(TRIM(F10&amp;" "&amp;G10&amp;" "&amp;H10)," ","-")</f>
         <v>form-description</v>
       </c>
-      <c r="U10" s="137" t="s">
-        <v>179</v>
-      </c>
-      <c r="V10" s="134" t="str">
+      <c r="U10" s="136" t="s">
+        <v>176</v>
+      </c>
+      <c r="V10" s="133" t="str">
         <f t="shared" ref="V10:V11" si="4">IF(M10="COMPLETE","false","true")</f>
         <v>true</v>
       </c>
@@ -33348,62 +33342,62 @@
     <row r="11" spans="1:37" ht="18" customHeight="1">
       <c r="A11" s="80"/>
       <c r="B11" s="85"/>
-      <c r="C11" s="119">
+      <c r="C11" s="118">
         <v>1</v>
       </c>
-      <c r="D11" s="119" t="s">
-        <v>133</v>
-      </c>
-      <c r="E11" s="119">
+      <c r="D11" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="118">
         <v>2</v>
       </c>
-      <c r="F11" s="121" t="s">
-        <v>169</v>
-      </c>
-      <c r="G11" s="123" t="s">
-        <v>173</v>
-      </c>
-      <c r="H11" s="123"/>
-      <c r="I11" s="126" t="s">
+      <c r="F11" s="120" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="122" t="s">
+        <v>170</v>
+      </c>
+      <c r="H11" s="122"/>
+      <c r="I11" s="125" t="s">
+        <v>179</v>
+      </c>
+      <c r="J11" s="127" t="s">
+        <v>180</v>
+      </c>
+      <c r="K11" s="125" t="s">
+        <v>181</v>
+      </c>
+      <c r="L11" s="125" t="s">
         <v>182</v>
       </c>
-      <c r="J11" s="128" t="s">
-        <v>183</v>
-      </c>
-      <c r="K11" s="126" t="s">
-        <v>184</v>
-      </c>
-      <c r="L11" s="126" t="s">
-        <v>185</v>
-      </c>
-      <c r="M11" s="130" t="str">
+      <c r="M11" s="129" t="str">
         <f t="shared" si="0"/>
         <v>Form\'s description cannot be empty</v>
       </c>
-      <c r="N11" s="131"/>
-      <c r="O11" s="131" t="s">
-        <v>178</v>
+      <c r="N11" s="130"/>
+      <c r="O11" s="130" t="s">
+        <v>175</v>
       </c>
       <c r="P11" s="74" t="str">
         <f t="shared" si="1"/>
         <v>"form[$form.getId()]","form.description","en","1.2 [form.description] - Form\'s description cannot be empty","Form\'s description cannot be empty","A name with some value different than empty","es","1.2 [form.description] - La descripción de la forma no pude ser vacío","La descripción de la forma no pude ser vacío","Una descripción con algún valor diferente de vacío",$form.getDescription(),$form.getId()</v>
       </c>
-      <c r="Q11" s="133" t="str">
+      <c r="Q11" s="132" t="str">
         <f t="shared" si="2"/>
         <v>"ERROR","Form\'s description cannot be empty"</v>
       </c>
-      <c r="R11" s="135"/>
-      <c r="S11" s="134" t="s">
+      <c r="R11" s="134"/>
+      <c r="S11" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="T11" s="137" t="str">
+      <c r="T11" s="136" t="str">
         <f t="shared" si="3"/>
         <v>form-description</v>
       </c>
-      <c r="U11" s="137" t="s">
-        <v>186</v>
-      </c>
-      <c r="V11" s="134" t="str">
+      <c r="U11" s="136" t="s">
+        <v>183</v>
+      </c>
+      <c r="V11" s="133" t="str">
         <f t="shared" si="4"/>
         <v>true</v>
       </c>
@@ -33427,30 +33421,30 @@
     </row>
     <row r="12" spans="1:37" ht="17.25" customHeight="1">
       <c r="A12" s="80"/>
-      <c r="B12" s="172" t="s">
-        <v>187</v>
-      </c>
-      <c r="C12" s="159"/>
-      <c r="D12" s="159"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="159"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="159"/>
-      <c r="I12" s="159"/>
-      <c r="J12" s="159"/>
-      <c r="K12" s="159"/>
-      <c r="L12" s="159"/>
-      <c r="M12" s="159"/>
-      <c r="N12" s="159"/>
-      <c r="O12" s="159"/>
-      <c r="P12" s="159"/>
-      <c r="Q12" s="159"/>
+      <c r="B12" s="161" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="162"/>
+      <c r="D12" s="162"/>
+      <c r="E12" s="162"/>
+      <c r="F12" s="162"/>
+      <c r="G12" s="162"/>
+      <c r="H12" s="162"/>
+      <c r="I12" s="162"/>
+      <c r="J12" s="162"/>
+      <c r="K12" s="162"/>
+      <c r="L12" s="162"/>
+      <c r="M12" s="162"/>
+      <c r="N12" s="162"/>
+      <c r="O12" s="162"/>
+      <c r="P12" s="162"/>
+      <c r="Q12" s="162"/>
       <c r="R12" s="81"/>
       <c r="S12" s="91"/>
       <c r="T12" s="91"/>
       <c r="U12" s="91"/>
       <c r="V12" s="91"/>
-      <c r="W12" s="139"/>
+      <c r="W12" s="138"/>
       <c r="X12" s="92"/>
       <c r="Y12" s="92"/>
       <c r="Z12" s="92"/>
@@ -33469,18 +33463,18 @@
     <row r="13" spans="1:37" ht="18">
       <c r="A13" s="80"/>
       <c r="B13" s="85"/>
-      <c r="C13" s="158" t="s">
+      <c r="C13" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="159"/>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="159"/>
-      <c r="L13" s="160"/>
+      <c r="D13" s="162"/>
+      <c r="E13" s="162"/>
+      <c r="F13" s="162"/>
+      <c r="G13" s="162"/>
+      <c r="H13" s="162"/>
+      <c r="I13" s="162"/>
+      <c r="J13" s="162"/>
+      <c r="K13" s="162"/>
+      <c r="L13" s="164"/>
       <c r="M13" s="86" t="s">
         <v>68</v>
       </c>
@@ -33530,23 +33524,23 @@
     <row r="14" spans="1:37" ht="18">
       <c r="A14" s="80"/>
       <c r="B14" s="85"/>
-      <c r="C14" s="162"/>
+      <c r="C14" s="168"/>
       <c r="D14" s="156"/>
       <c r="E14" s="156"/>
       <c r="F14" s="156"/>
       <c r="G14" s="156"/>
-      <c r="H14" s="163"/>
+      <c r="H14" s="169"/>
       <c r="I14" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="J14" s="167"/>
+      <c r="J14" s="172"/>
       <c r="K14" s="166" t="s">
         <v>94</v>
       </c>
-      <c r="L14" s="168"/>
+      <c r="L14" s="167"/>
       <c r="M14" s="94"/>
       <c r="N14" s="174" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O14" s="176"/>
       <c r="P14" s="96"/>
@@ -33575,28 +33569,28 @@
     <row r="15" spans="1:37" ht="18" customHeight="1">
       <c r="A15" s="80"/>
       <c r="B15" s="85"/>
-      <c r="C15" s="164"/>
-      <c r="D15" s="164"/>
-      <c r="E15" s="164"/>
-      <c r="F15" s="164"/>
-      <c r="G15" s="164"/>
-      <c r="H15" s="165"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="170"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="170"/>
+      <c r="G15" s="170"/>
+      <c r="H15" s="171"/>
       <c r="I15" s="99"/>
       <c r="J15" s="100"/>
       <c r="K15" s="101"/>
-      <c r="L15" s="104"/>
+      <c r="L15" s="103"/>
       <c r="M15" s="94"/>
-      <c r="N15" s="105" t="s">
-        <v>188</v>
-      </c>
-      <c r="O15" s="149" t="s">
-        <v>189</v>
-      </c>
-      <c r="P15" s="103" t="s">
-        <v>166</v>
+      <c r="N15" s="104" t="s">
+        <v>185</v>
+      </c>
+      <c r="O15" s="148" t="s">
+        <v>186</v>
+      </c>
+      <c r="P15" s="102" t="s">
+        <v>163</v>
       </c>
       <c r="Q15" s="56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R15" s="97"/>
       <c r="S15" s="89"/>
@@ -33622,47 +33616,47 @@
     <row r="16" spans="1:37" ht="18">
       <c r="A16" s="80"/>
       <c r="B16" s="85"/>
-      <c r="C16" s="169" t="s">
+      <c r="C16" s="158" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="105" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="170"/>
-      <c r="E16" s="170"/>
-      <c r="F16" s="170"/>
-      <c r="G16" s="170"/>
-      <c r="H16" s="171"/>
-      <c r="I16" s="106" t="s">
+      <c r="J16" s="106" t="s">
         <v>124</v>
       </c>
-      <c r="J16" s="107" t="s">
+      <c r="K16" s="107" t="s">
         <v>125</v>
       </c>
-      <c r="K16" s="108" t="s">
+      <c r="L16" s="105" t="s">
         <v>126</v>
       </c>
-      <c r="L16" s="106" t="s">
+      <c r="M16" s="109" t="s">
         <v>127</v>
       </c>
-      <c r="M16" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="N16" s="110" t="s">
-        <v>167</v>
-      </c>
-      <c r="O16" s="110" t="s">
-        <v>168</v>
-      </c>
-      <c r="P16" s="112" t="s">
-        <v>130</v>
+      <c r="N16" s="109" t="s">
+        <v>164</v>
+      </c>
+      <c r="O16" s="109" t="s">
+        <v>165</v>
+      </c>
+      <c r="P16" s="111" t="s">
+        <v>129</v>
       </c>
       <c r="Q16" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="R16" s="150"/>
-      <c r="S16" s="114"/>
-      <c r="T16" s="114"/>
-      <c r="U16" s="114"/>
-      <c r="V16" s="114"/>
-      <c r="W16" s="114"/>
+        <v>131</v>
+      </c>
+      <c r="R16" s="149"/>
+      <c r="S16" s="113"/>
+      <c r="T16" s="113"/>
+      <c r="U16" s="113"/>
+      <c r="V16" s="113"/>
+      <c r="W16" s="113"/>
       <c r="X16" s="90"/>
       <c r="Y16" s="90"/>
       <c r="Z16" s="90"/>
@@ -33681,60 +33675,60 @@
     <row r="17" spans="1:37" ht="18.75" customHeight="1">
       <c r="A17" s="80"/>
       <c r="B17" s="85"/>
-      <c r="C17" s="119">
+      <c r="C17" s="118">
         <v>2</v>
       </c>
-      <c r="D17" s="119" t="s">
-        <v>133</v>
-      </c>
-      <c r="E17" s="119">
+      <c r="D17" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="118">
         <v>1</v>
       </c>
-      <c r="F17" s="121" t="s">
+      <c r="F17" s="120" t="s">
+        <v>187</v>
+      </c>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="125" t="s">
+        <v>188</v>
+      </c>
+      <c r="J17" s="125" t="s">
+        <v>189</v>
+      </c>
+      <c r="K17" s="125" t="s">
         <v>190</v>
       </c>
-      <c r="G17" s="125"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="126" t="s">
+      <c r="L17" s="125" t="s">
         <v>191</v>
       </c>
-      <c r="J17" s="126" t="s">
-        <v>192</v>
-      </c>
-      <c r="K17" s="126" t="s">
-        <v>193</v>
-      </c>
-      <c r="L17" s="126" t="s">
-        <v>194</v>
-      </c>
-      <c r="M17" s="130" t="str">
+      <c r="M17" s="129" t="str">
         <f t="shared" ref="M17:M18" si="5">I17</f>
         <v>Form\'s questions cannot be null</v>
       </c>
-      <c r="N17" s="131" t="s">
-        <v>178</v>
-      </c>
-      <c r="O17" s="151"/>
+      <c r="N17" s="130" t="s">
+        <v>175</v>
+      </c>
+      <c r="O17" s="150"/>
       <c r="P17" s="74" t="str">
         <f t="shared" ref="P17:P18" si="6">CONCATENATE("""",CONCATENATE("form[","$form.getId()","]"),"""",",","""",SUBSTITUTE(TRIM(F17&amp;" "&amp;G17&amp;" "&amp;H17)," ","."),"""",",","""",$I$7,"""",",","""",CONCATENATE(C17,D17,E17)," [",SUBSTITUTE(TRIM(F17&amp;" "&amp;G17&amp;" "&amp;H17)," ","."),"] - ",I17,"""",",","""",I17,"""",",","""",J17,"""",",","""", $K$7,"""",",","""",CONCATENATE(C17,D17,E17)," [",SUBSTITUTE(TRIM(F17&amp;" "&amp;G17&amp;" "&amp;H17)," ","."),"] - ",K17,"""",",","""",K17,"""",",","""",L17,"""",",","$form.getQuestions()",",","$form.getId()")</f>
         <v>"form[$form.getId()]","question","en","2.1 [question] - Form\'s questions cannot be null","Form\'s questions cannot be null","An question list with some value different than null","es","2.1 [question] - Las preguntas de la forma no pueden ser nulas","Las preguntas de la forma no pueden ser nulas","Un listado de preguntas diferente de nulo",$form.getQuestions(),$form.getId()</v>
       </c>
-      <c r="Q17" s="133" t="str">
+      <c r="Q17" s="132" t="str">
         <f t="shared" ref="Q17:Q18" si="7">CONCATENATE("""","ERROR","""",",","""",I17,"""")</f>
         <v>"ERROR","Form\'s questions cannot be null"</v>
       </c>
-      <c r="R17" s="135"/>
-      <c r="S17" s="134" t="s">
+      <c r="R17" s="134"/>
+      <c r="S17" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="T17" s="137" t="str">
+      <c r="T17" s="136" t="str">
         <f t="shared" ref="T17:T18" si="8">SUBSTITUTE(TRIM(F17&amp;" "&amp;G17&amp;" "&amp;H17)," ","-")</f>
         <v>question</v>
       </c>
-      <c r="U17" s="152" t="s">
-        <v>195</v>
-      </c>
-      <c r="V17" s="134" t="str">
+      <c r="U17" s="151" t="s">
+        <v>192</v>
+      </c>
+      <c r="V17" s="133" t="str">
         <f t="shared" ref="V17:V18" si="9">IF(N17="COMPLETE","false","true")</f>
         <v>true</v>
       </c>
@@ -33759,60 +33753,60 @@
     <row r="18" spans="1:37" ht="17.25" customHeight="1">
       <c r="A18" s="80"/>
       <c r="B18" s="85"/>
-      <c r="C18" s="119">
+      <c r="C18" s="118">
         <v>2</v>
       </c>
-      <c r="D18" s="119" t="s">
-        <v>133</v>
-      </c>
-      <c r="E18" s="119">
+      <c r="D18" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="118">
         <v>2</v>
       </c>
-      <c r="F18" s="121" t="s">
-        <v>190</v>
-      </c>
-      <c r="G18" s="125"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="126" t="s">
+      <c r="F18" s="120" t="s">
+        <v>187</v>
+      </c>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="125" t="s">
+        <v>194</v>
+      </c>
+      <c r="J18" s="125" t="s">
+        <v>195</v>
+      </c>
+      <c r="K18" s="125" t="s">
+        <v>196</v>
+      </c>
+      <c r="L18" s="125" t="s">
         <v>197</v>
       </c>
-      <c r="J18" s="126" t="s">
-        <v>198</v>
-      </c>
-      <c r="K18" s="126" t="s">
-        <v>199</v>
-      </c>
-      <c r="L18" s="126" t="s">
-        <v>200</v>
-      </c>
-      <c r="M18" s="130" t="str">
+      <c r="M18" s="129" t="str">
         <f t="shared" si="5"/>
         <v>Form\'s questions cannot be empty</v>
       </c>
-      <c r="N18" s="154"/>
-      <c r="O18" s="131" t="s">
-        <v>178</v>
+      <c r="N18" s="153"/>
+      <c r="O18" s="130" t="s">
+        <v>175</v>
       </c>
       <c r="P18" s="74" t="str">
         <f t="shared" si="6"/>
         <v>"form[$form.getId()]","question","en","2.2 [question] - Form\'s questions cannot be empty","Form\'s questions cannot be empty","An question list with some value different than empty","es","2.2 [question] - Las preguntas de la forma no pueden ser vacías","Las preguntas de la forma no pueden ser vacías","Un listado de preguntas diferente de vacío",$form.getQuestions(),$form.getId()</v>
       </c>
-      <c r="Q18" s="133" t="str">
+      <c r="Q18" s="132" t="str">
         <f t="shared" si="7"/>
         <v>"ERROR","Form\'s questions cannot be empty"</v>
       </c>
-      <c r="R18" s="135"/>
-      <c r="S18" s="134" t="s">
+      <c r="R18" s="134"/>
+      <c r="S18" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="T18" s="137" t="str">
+      <c r="T18" s="136" t="str">
         <f t="shared" si="8"/>
         <v>question</v>
       </c>
-      <c r="U18" s="152" t="s">
-        <v>201</v>
-      </c>
-      <c r="V18" s="134" t="str">
+      <c r="U18" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="V18" s="133" t="str">
         <f t="shared" si="9"/>
         <v>true</v>
       </c>
@@ -33870,8 +33864,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="150" customHeight="1">
-      <c r="A1" s="153" t="s">
-        <v>196</v>
+      <c r="A1" s="152" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>